<commit_message>
added a bunch of features... need to fix a bunch of bugs
</commit_message>
<xml_diff>
--- a/advertising-packets.xlsx
+++ b/advertising-packets.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6160" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21880" windowHeight="28260" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="42">
   <si>
     <t>time</t>
   </si>
@@ -117,22 +118,40 @@
     <t>lsm9setting</t>
   </si>
   <si>
-    <t>click/turn</t>
-  </si>
-  <si>
-    <t>mm/turn</t>
-  </si>
-  <si>
-    <t>bits</t>
+    <t>packet type + setting</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>wheel</t>
+  </si>
+  <si>
+    <t>zero pos</t>
+  </si>
+  <si>
+    <t>tb0</t>
+  </si>
+  <si>
+    <t>tb1</t>
+  </si>
+  <si>
+    <t>tb2</t>
+  </si>
+  <si>
+    <t>humidity</t>
+  </si>
+  <si>
+    <t>air pressure</t>
+  </si>
+  <si>
+    <t>temp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0000000"/>
-  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -175,7 +194,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -185,20 +204,59 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="29">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -528,43 +586,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:10">
       <c r="B1" t="s">
         <v>29</v>
       </c>
+      <c r="C1">
+        <v>0</v>
+      </c>
       <c r="D1" t="s">
         <v>30</v>
       </c>
-      <c r="F1">
+      <c r="G1">
+        <v>0</v>
+      </c>
+      <c r="H1">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="I1">
+        <v>2</v>
+      </c>
+      <c r="J1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="B2" t="s">
         <v>31</v>
       </c>
       <c r="D2" t="s">
         <v>30</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>0</v>
       </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>0</v>
       </c>
@@ -577,14 +645,11 @@
       <c r="D3" t="s">
         <v>1</v>
       </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
       <c r="F3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4">
         <v>1</v>
       </c>
@@ -597,14 +662,23 @@
       <c r="D4" t="s">
         <v>5</v>
       </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
       <c r="F4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:12">
+      <c r="G4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5">
         <v>2</v>
       </c>
@@ -617,14 +691,20 @@
       <c r="D5" t="s">
         <v>5</v>
       </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
       <c r="F5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
+        <v>3</v>
+      </c>
+      <c r="H5" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5" t="s">
+        <v>36</v>
+      </c>
+      <c r="J5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6">
         <v>3</v>
       </c>
@@ -637,18 +717,20 @@
       <c r="D6" t="s">
         <v>5</v>
       </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
       <c r="F6">
-        <v>2</v>
-      </c>
-      <c r="I6">
-        <f>I8/I7</f>
-        <v>1.27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
+        <v>4</v>
+      </c>
+      <c r="H6" t="s">
+        <v>37</v>
+      </c>
+      <c r="I6" t="s">
+        <v>37</v>
+      </c>
+      <c r="J6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7">
         <v>4</v>
       </c>
@@ -661,20 +743,20 @@
       <c r="D7" t="s">
         <v>5</v>
       </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
       <c r="F7">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H7" t="s">
-        <v>32</v>
-      </c>
-      <c r="I7">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
+        <v>38</v>
+      </c>
+      <c r="I7" t="s">
+        <v>38</v>
+      </c>
+      <c r="J7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8">
         <v>5</v>
       </c>
@@ -687,20 +769,20 @@
       <c r="D8" t="s">
         <v>5</v>
       </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
       <c r="F8">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H8" t="s">
-        <v>33</v>
-      </c>
-      <c r="I8">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
+        <v>39</v>
+      </c>
+      <c r="I8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9">
         <v>6</v>
       </c>
@@ -713,20 +795,20 @@
       <c r="D9" t="s">
         <v>5</v>
       </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
       <c r="F9">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H9" t="s">
-        <v>34</v>
-      </c>
-      <c r="I9">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
+        <v>39</v>
+      </c>
+      <c r="I9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10">
         <v>7</v>
       </c>
@@ -739,25 +821,20 @@
       <c r="D10" t="s">
         <v>5</v>
       </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
       <c r="F10">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="H10" t="s">
-        <v>18</v>
-      </c>
-      <c r="I10">
-        <f>2^I9/I7*I8/1000</f>
-        <v>83.230720000000005</v>
-      </c>
-      <c r="L10" s="1">
-        <f>10*2.54*0.01 / 200</f>
-        <v>1.2700000000000001E-3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
+        <v>39</v>
+      </c>
+      <c r="I10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11">
         <v>8</v>
       </c>
@@ -770,14 +847,20 @@
       <c r="D11" t="s">
         <v>5</v>
       </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
       <c r="F11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
+        <v>9</v>
+      </c>
+      <c r="H11" t="s">
+        <v>39</v>
+      </c>
+      <c r="I11" t="s">
+        <v>17</v>
+      </c>
+      <c r="J11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12">
         <v>9</v>
       </c>
@@ -790,14 +873,20 @@
       <c r="D12" t="s">
         <v>5</v>
       </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
       <c r="F12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
+        <v>10</v>
+      </c>
+      <c r="H12" t="s">
+        <v>40</v>
+      </c>
+      <c r="I12" t="s">
+        <v>25</v>
+      </c>
+      <c r="J12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13">
         <v>10</v>
       </c>
@@ -810,14 +899,20 @@
       <c r="D13" t="s">
         <v>5</v>
       </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
       <c r="F13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
+        <v>11</v>
+      </c>
+      <c r="H13" t="s">
+        <v>40</v>
+      </c>
+      <c r="I13" t="s">
+        <v>25</v>
+      </c>
+      <c r="J13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14">
         <v>11</v>
       </c>
@@ -830,14 +925,20 @@
       <c r="D14" t="s">
         <v>5</v>
       </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
       <c r="F14">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
+        <v>12</v>
+      </c>
+      <c r="H14" t="s">
+        <v>40</v>
+      </c>
+      <c r="I14" t="s">
+        <v>25</v>
+      </c>
+      <c r="J14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15">
         <v>12</v>
       </c>
@@ -850,14 +951,20 @@
       <c r="D15" t="s">
         <v>14</v>
       </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
       <c r="F15">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
+        <v>13</v>
+      </c>
+      <c r="H15" t="s">
+        <v>40</v>
+      </c>
+      <c r="I15" t="s">
+        <v>25</v>
+      </c>
+      <c r="J15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16">
         <v>13</v>
       </c>
@@ -870,14 +977,20 @@
       <c r="D16" t="s">
         <v>5</v>
       </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
       <c r="F16">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+        <v>14</v>
+      </c>
+      <c r="H16" t="s">
+        <v>41</v>
+      </c>
+      <c r="I16" t="s">
+        <v>26</v>
+      </c>
+      <c r="J16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17">
         <v>14</v>
       </c>
@@ -890,14 +1003,20 @@
       <c r="D17" t="s">
         <v>5</v>
       </c>
-      <c r="E17">
-        <v>2</v>
-      </c>
       <c r="F17">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+        <v>15</v>
+      </c>
+      <c r="H17" t="s">
+        <v>41</v>
+      </c>
+      <c r="I17" t="s">
+        <v>26</v>
+      </c>
+      <c r="J17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18">
         <v>15</v>
       </c>
@@ -910,14 +1029,20 @@
       <c r="D18" t="s">
         <v>5</v>
       </c>
-      <c r="E18">
-        <v>2</v>
-      </c>
       <c r="F18">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+        <v>16</v>
+      </c>
+      <c r="H18" t="s">
+        <v>41</v>
+      </c>
+      <c r="I18" t="s">
+        <v>26</v>
+      </c>
+      <c r="J18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19">
         <v>16</v>
       </c>
@@ -930,11 +1055,72 @@
       <c r="D19" t="s">
         <v>5</v>
       </c>
-      <c r="E19">
-        <v>2</v>
-      </c>
       <c r="F19">
-        <v>4</v>
+        <v>17</v>
+      </c>
+      <c r="H19" t="s">
+        <v>41</v>
+      </c>
+      <c r="I19" t="s">
+        <v>26</v>
+      </c>
+      <c r="J19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="F20">
+        <v>18</v>
+      </c>
+      <c r="J20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="F21">
+        <v>19</v>
+      </c>
+      <c r="J21" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="F22">
+        <v>20</v>
+      </c>
+      <c r="J22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="F23">
+        <v>21</v>
+      </c>
+      <c r="J23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="F24">
+        <v>22</v>
+      </c>
+      <c r="J24" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="F25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="F26">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="F27">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -946,4 +1132,21 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
A boatload of refactoring
</commit_message>
<xml_diff>
--- a/advertising-packets.xlsx
+++ b/advertising-packets.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="51200" windowHeight="28800" tabRatio="500"/>
+    <workbookView xWindow="4180" yWindow="2920" windowWidth="35400" windowHeight="28260" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Bytes" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="116">
   <si>
     <t>packet type + setting</t>
   </si>
@@ -190,18 +190,6 @@
     <t>0x01 Cypress Bluetooth ID byte 1</t>
   </si>
   <si>
-    <t>Packet 0</t>
-  </si>
-  <si>
-    <t>Packet 1</t>
-  </si>
-  <si>
-    <t>Packet 2</t>
-  </si>
-  <si>
-    <t>Packet 3</t>
-  </si>
-  <si>
     <t>Altitude Float byte 0</t>
   </si>
   <si>
@@ -371,6 +359,15 @@
   </si>
   <si>
     <t>Reset position of cart in Clicks</t>
+  </si>
+  <si>
+    <t>Packet 0 (Kinematic)</t>
+  </si>
+  <si>
+    <t>Packet 1 (Enviro)</t>
+  </si>
+  <si>
+    <t>Packet 2 (Admin)</t>
   </si>
 </sst>
 </file>
@@ -434,8 +431,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="109">
+  <cellStyleXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -558,7 +557,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="109">
+  <cellStyles count="111">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -613,6 +612,7 @@
     <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -667,6 +667,7 @@
     <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -996,38 +997,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="220" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17:D22"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B1" t="s">
-        <v>56</v>
+        <v>113</v>
       </c>
       <c r="C1" t="s">
-        <v>57</v>
+        <v>114</v>
       </c>
       <c r="D1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1040,11 +1037,8 @@
       <c r="D2" t="s">
         <v>54</v>
       </c>
-      <c r="E2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1057,11 +1051,8 @@
       <c r="D3" t="s">
         <v>55</v>
       </c>
-      <c r="E3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1074,11 +1065,8 @@
       <c r="D4" t="s">
         <v>0</v>
       </c>
-      <c r="E4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1089,13 +1077,10 @@
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1106,13 +1091,10 @@
         <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:4">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1123,13 +1105,10 @@
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:4">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1140,13 +1119,10 @@
         <v>42</v>
       </c>
       <c r="D8" t="s">
-        <v>60</v>
-      </c>
-      <c r="E8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:4">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1157,13 +1133,10 @@
         <v>43</v>
       </c>
       <c r="D9" t="s">
-        <v>61</v>
-      </c>
-      <c r="E9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:4">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1174,13 +1147,10 @@
         <v>44</v>
       </c>
       <c r="D10" t="s">
-        <v>62</v>
-      </c>
-      <c r="E10" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:4">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1191,13 +1161,10 @@
         <v>45</v>
       </c>
       <c r="D11" t="s">
-        <v>63</v>
-      </c>
-      <c r="E11" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:4">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1208,13 +1175,10 @@
         <v>46</v>
       </c>
       <c r="D12" t="s">
-        <v>82</v>
-      </c>
-      <c r="E12" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:4">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1225,13 +1189,10 @@
         <v>47</v>
       </c>
       <c r="D13" t="s">
-        <v>82</v>
-      </c>
-      <c r="E13" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:4">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1242,13 +1203,10 @@
         <v>48</v>
       </c>
       <c r="D14" t="s">
-        <v>82</v>
-      </c>
-      <c r="E14" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:4">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1259,13 +1217,10 @@
         <v>49</v>
       </c>
       <c r="D15" t="s">
-        <v>82</v>
-      </c>
-      <c r="E15" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:4">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1276,13 +1231,10 @@
         <v>50</v>
       </c>
       <c r="D16" t="s">
-        <v>82</v>
-      </c>
-      <c r="E16" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:4">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1293,13 +1245,10 @@
         <v>51</v>
       </c>
       <c r="D17" t="s">
-        <v>82</v>
-      </c>
-      <c r="E17" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:4">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1310,13 +1259,10 @@
         <v>52</v>
       </c>
       <c r="D18" t="s">
-        <v>82</v>
-      </c>
-      <c r="E18" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1327,13 +1273,10 @@
         <v>53</v>
       </c>
       <c r="D19" t="s">
-        <v>82</v>
-      </c>
-      <c r="E19" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:4">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1341,16 +1284,13 @@
         <v>16</v>
       </c>
       <c r="C20" t="s">
-        <v>82</v>
+        <v>56</v>
       </c>
       <c r="D20" t="s">
-        <v>82</v>
-      </c>
-      <c r="E20" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:4">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1358,16 +1298,13 @@
         <v>17</v>
       </c>
       <c r="C21" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="D21" t="s">
-        <v>82</v>
-      </c>
-      <c r="E21" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:4">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1375,16 +1312,13 @@
         <v>19</v>
       </c>
       <c r="C22" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="D22" t="s">
-        <v>82</v>
-      </c>
-      <c r="E22" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:4">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1392,16 +1326,13 @@
         <v>20</v>
       </c>
       <c r="C23" t="s">
-        <v>82</v>
+        <v>59</v>
       </c>
       <c r="D23" t="s">
-        <v>82</v>
-      </c>
-      <c r="E23" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:4">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1409,16 +1340,13 @@
         <v>21</v>
       </c>
       <c r="C24" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D24" t="s">
-        <v>82</v>
-      </c>
-      <c r="E24" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:4">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1426,16 +1354,13 @@
         <v>22</v>
       </c>
       <c r="C25" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D25" t="s">
-        <v>82</v>
-      </c>
-      <c r="E25" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26">
         <v>24</v>
       </c>
@@ -1443,16 +1368,13 @@
         <v>23</v>
       </c>
       <c r="C26" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D26" t="s">
-        <v>82</v>
-      </c>
-      <c r="E26" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27">
         <v>25</v>
       </c>
@@ -1460,13 +1382,10 @@
         <v>24</v>
       </c>
       <c r="C27" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D27" t="s">
-        <v>82</v>
-      </c>
-      <c r="E27" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1501,22 +1420,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>67</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1527,16 +1446,16 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E2">
         <v>2</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="105">
@@ -1547,13 +1466,13 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1564,16 +1483,16 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" t="s">
         <v>70</v>
-      </c>
-      <c r="D4" t="s">
-        <v>74</v>
       </c>
       <c r="E4">
         <v>3</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="45">
@@ -1584,16 +1503,16 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" t="s">
         <v>72</v>
       </c>
-      <c r="D5" t="s">
-        <v>76</v>
-      </c>
       <c r="E5">
         <v>2</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="75">
@@ -1604,16 +1523,16 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" t="s">
         <v>73</v>
       </c>
-      <c r="D6" t="s">
-        <v>77</v>
-      </c>
       <c r="E6">
         <v>2</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1624,16 +1543,16 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D7" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E7">
         <v>2</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1644,16 +1563,16 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>79</v>
-      </c>
-      <c r="D8" t="s">
-        <v>77</v>
-      </c>
-      <c r="E8">
-        <v>2</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1664,16 +1583,16 @@
         <v>14</v>
       </c>
       <c r="C9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9" t="s">
+        <v>73</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>86</v>
-      </c>
-      <c r="D9" t="s">
-        <v>77</v>
-      </c>
-      <c r="E9">
-        <v>2</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1684,16 +1603,16 @@
         <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D10" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E10">
         <v>2</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1704,16 +1623,16 @@
         <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D11" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E11">
         <v>2</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1724,16 +1643,16 @@
         <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D12" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E12">
         <v>2</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1744,16 +1663,16 @@
         <v>22</v>
       </c>
       <c r="C13" t="s">
+        <v>83</v>
+      </c>
+      <c r="D13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13" s="4" t="s">
         <v>87</v>
-      </c>
-      <c r="D13" t="s">
-        <v>77</v>
-      </c>
-      <c r="E13">
-        <v>2</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1764,16 +1683,16 @@
         <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D14" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E14">
         <v>2</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1784,16 +1703,16 @@
         <v>0</v>
       </c>
       <c r="C15" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D15" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E15">
         <v>2</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="105">
@@ -1804,13 +1723,13 @@
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E16">
         <v>1</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1821,16 +1740,16 @@
         <v>3</v>
       </c>
       <c r="C17" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" t="s">
         <v>70</v>
-      </c>
-      <c r="D17" t="s">
-        <v>74</v>
       </c>
       <c r="E17">
         <v>3</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1841,16 +1760,16 @@
         <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D18" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E18">
         <v>4</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1861,16 +1780,16 @@
         <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D19" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E19">
         <v>4</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1881,16 +1800,16 @@
         <v>14</v>
       </c>
       <c r="C20" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D20" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E20">
         <v>4</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1901,16 +1820,16 @@
         <v>0</v>
       </c>
       <c r="C21" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D21" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E21">
         <v>2</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="105">
@@ -1921,13 +1840,13 @@
         <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E22">
         <v>1</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1938,16 +1857,16 @@
         <v>3</v>
       </c>
       <c r="C23" t="s">
+        <v>66</v>
+      </c>
+      <c r="D23" t="s">
         <v>70</v>
-      </c>
-      <c r="D23" t="s">
-        <v>74</v>
       </c>
       <c r="E23">
         <v>3</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1958,16 +1877,16 @@
         <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D24" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E24">
         <v>4</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1978,16 +1897,16 @@
         <v>10</v>
       </c>
       <c r="C25" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D25" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E25">
         <v>4</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1998,16 +1917,16 @@
         <v>14</v>
       </c>
       <c r="C26" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D26" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E26">
         <v>4</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -2018,16 +1937,16 @@
         <v>0</v>
       </c>
       <c r="C27" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D27" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E27">
         <v>2</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="105">
@@ -2038,13 +1957,13 @@
         <v>2</v>
       </c>
       <c r="C28" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E28">
         <v>1</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -2055,16 +1974,16 @@
         <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D29" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E29">
         <v>14</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -2075,16 +1994,16 @@
         <v>19</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D30" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E30">
         <v>4</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -2095,16 +2014,16 @@
         <v>21</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D31" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E31">
         <v>2</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
a shitload of updates
</commit_message>
<xml_diff>
--- a/advertising-packets.xlsx
+++ b/advertising-packets.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="36220" windowHeight="25980" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Bytes" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="119">
   <si>
     <t>packet type + setting</t>
   </si>
@@ -371,6 +371,12 @@
   </si>
   <si>
     <t>zero pos (16-bit unsigned int byte 1)</t>
+  </si>
+  <si>
+    <t>Ticks/Rotation (16-bit unsigned int byte0)</t>
+  </si>
+  <si>
+    <t>Ticks/Rotation (16-bit unsigned int byte1)</t>
   </si>
 </sst>
 </file>
@@ -434,8 +440,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="113">
+  <cellStyleXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -562,7 +570,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="113">
+  <cellStyles count="115">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -619,6 +627,7 @@
     <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -675,6 +684,7 @@
     <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1006,8 +1016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="220" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12:C15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="220" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1364,7 +1374,7 @@
         <v>77</v>
       </c>
       <c r="D25" t="s">
-        <v>77</v>
+        <v>117</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1378,7 +1388,7 @@
         <v>77</v>
       </c>
       <c r="D26" t="s">
-        <v>77</v>
+        <v>118</v>
       </c>
     </row>
     <row r="27" spans="1:4">

</xml_diff>

<commit_message>
first revision of demo mode
</commit_message>
<xml_diff>
--- a/advertising-packets.xlsx
+++ b/advertising-packets.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28260" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Bytes" sheetId="1" r:id="rId1"/>
@@ -157,18 +157,6 @@
     <t>Humidity Float byte 3</t>
   </si>
   <si>
-    <t>Air Pressure Float Byte 0</t>
-  </si>
-  <si>
-    <t>Air Pressure Float Byte 1</t>
-  </si>
-  <si>
-    <t>Air Pressure Float Byte 2</t>
-  </si>
-  <si>
-    <t>Air Pressure Float Byte 3</t>
-  </si>
-  <si>
     <t>Temperature Float Byte 0</t>
   </si>
   <si>
@@ -377,6 +365,18 @@
   </si>
   <si>
     <t>Ticks/Rotation (16-bit unsigned int byte1)</t>
+  </si>
+  <si>
+    <t>Air Pressure Int Byte 0</t>
+  </si>
+  <si>
+    <t>Air Pressure Int Byte 1</t>
+  </si>
+  <si>
+    <t>Air Pressure Int Byte 2</t>
+  </si>
+  <si>
+    <t>Air Pressure Int Byte 3</t>
   </si>
 </sst>
 </file>
@@ -1016,8 +1016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="220" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="220" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1029,16 +1029,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1046,13 +1046,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1060,13 +1060,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1189,7 +1189,7 @@
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>45</v>
+        <v>115</v>
       </c>
       <c r="D12" t="s">
         <v>34</v>
@@ -1203,7 +1203,7 @@
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>46</v>
+        <v>116</v>
       </c>
       <c r="D13" t="s">
         <v>35</v>
@@ -1217,7 +1217,7 @@
         <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>47</v>
+        <v>117</v>
       </c>
       <c r="D14" t="s">
         <v>36</v>
@@ -1231,7 +1231,7 @@
         <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>48</v>
+        <v>118</v>
       </c>
       <c r="D15" t="s">
         <v>37</v>
@@ -1245,7 +1245,7 @@
         <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D16" t="s">
         <v>38</v>
@@ -1259,7 +1259,7 @@
         <v>12</v>
       </c>
       <c r="C17" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D17" t="s">
         <v>39</v>
@@ -1273,10 +1273,10 @@
         <v>13</v>
       </c>
       <c r="C18" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D18" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1287,7 +1287,7 @@
         <v>14</v>
       </c>
       <c r="C19" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D19" t="s">
         <v>24</v>
@@ -1301,7 +1301,7 @@
         <v>15</v>
       </c>
       <c r="C20" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D20" t="s">
         <v>25</v>
@@ -1315,7 +1315,7 @@
         <v>16</v>
       </c>
       <c r="C21" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D21" t="s">
         <v>26</v>
@@ -1329,7 +1329,7 @@
         <v>18</v>
       </c>
       <c r="C22" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D22" t="s">
         <v>27</v>
@@ -1343,10 +1343,10 @@
         <v>19</v>
       </c>
       <c r="C23" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D23" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1357,10 +1357,10 @@
         <v>20</v>
       </c>
       <c r="C24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D24" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1371,10 +1371,10 @@
         <v>21</v>
       </c>
       <c r="C25" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D25" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1385,10 +1385,10 @@
         <v>22</v>
       </c>
       <c r="C26" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D26" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1399,10 +1399,10 @@
         <v>23</v>
       </c>
       <c r="C27" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D27" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1437,22 +1437,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1463,16 +1463,16 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E2">
         <v>2</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="105">
@@ -1483,13 +1483,13 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1500,16 +1500,16 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" t="s">
         <v>65</v>
-      </c>
-      <c r="D4" t="s">
-        <v>69</v>
       </c>
       <c r="E4">
         <v>3</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="45">
@@ -1520,16 +1520,16 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" t="s">
         <v>67</v>
       </c>
-      <c r="D5" t="s">
-        <v>71</v>
-      </c>
       <c r="E5">
         <v>2</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="75">
@@ -1540,16 +1540,16 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" t="s">
         <v>68</v>
       </c>
-      <c r="D6" t="s">
-        <v>72</v>
-      </c>
       <c r="E6">
         <v>2</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1560,16 +1560,16 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D7" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E7">
         <v>2</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1580,16 +1580,16 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" t="s">
+        <v>68</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>74</v>
-      </c>
-      <c r="D8" t="s">
-        <v>72</v>
-      </c>
-      <c r="E8">
-        <v>2</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1600,16 +1600,16 @@
         <v>14</v>
       </c>
       <c r="C9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D9" t="s">
+        <v>68</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>81</v>
-      </c>
-      <c r="D9" t="s">
-        <v>72</v>
-      </c>
-      <c r="E9">
-        <v>2</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1620,16 +1620,16 @@
         <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D10" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E10">
         <v>2</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1640,16 +1640,16 @@
         <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D11" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E11">
         <v>2</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1660,16 +1660,16 @@
         <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D12" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E12">
         <v>2</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1680,16 +1680,16 @@
         <v>22</v>
       </c>
       <c r="C13" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13" s="4" t="s">
         <v>82</v>
-      </c>
-      <c r="D13" t="s">
-        <v>72</v>
-      </c>
-      <c r="E13">
-        <v>2</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1700,16 +1700,16 @@
         <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D14" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E14">
         <v>2</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1720,16 +1720,16 @@
         <v>0</v>
       </c>
       <c r="C15" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D15" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E15">
         <v>2</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="105">
@@ -1740,13 +1740,13 @@
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E16">
         <v>1</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1757,16 +1757,16 @@
         <v>3</v>
       </c>
       <c r="C17" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" t="s">
         <v>65</v>
-      </c>
-      <c r="D17" t="s">
-        <v>69</v>
       </c>
       <c r="E17">
         <v>3</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1777,16 +1777,16 @@
         <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D18" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E18">
         <v>4</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1797,16 +1797,16 @@
         <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D19" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E19">
         <v>4</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1817,16 +1817,16 @@
         <v>14</v>
       </c>
       <c r="C20" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D20" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E20">
         <v>4</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1837,16 +1837,16 @@
         <v>0</v>
       </c>
       <c r="C21" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D21" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E21">
         <v>2</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="105">
@@ -1857,13 +1857,13 @@
         <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E22">
         <v>1</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1874,16 +1874,16 @@
         <v>3</v>
       </c>
       <c r="C23" t="s">
+        <v>61</v>
+      </c>
+      <c r="D23" t="s">
         <v>65</v>
-      </c>
-      <c r="D23" t="s">
-        <v>69</v>
       </c>
       <c r="E23">
         <v>3</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1894,16 +1894,16 @@
         <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D24" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E24">
         <v>4</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1914,16 +1914,16 @@
         <v>10</v>
       </c>
       <c r="C25" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D25" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E25">
         <v>4</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1934,16 +1934,16 @@
         <v>14</v>
       </c>
       <c r="C26" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D26" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E26">
         <v>4</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1954,16 +1954,16 @@
         <v>0</v>
       </c>
       <c r="C27" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D27" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E27">
         <v>2</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="105">
@@ -1974,13 +1974,13 @@
         <v>2</v>
       </c>
       <c r="C28" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E28">
         <v>1</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1991,16 +1991,16 @@
         <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D29" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E29">
         <v>14</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -2011,16 +2011,16 @@
         <v>19</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D30" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E30">
         <v>4</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -2031,16 +2031,16 @@
         <v>21</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D31" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E31">
         <v>2</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>